<commit_message>
viz updates, three more langs added for llama
</commit_message>
<xml_diff>
--- a/notebooks/viz/fact-completion-benchmark-results.xlsx
+++ b/notebooks/viz/fact-completion-benchmark-results.xlsx
@@ -618,9 +618,11 @@
         <v>17</v>
       </c>
       <c r="B16" s="4">
-        <v>10.0</v>
-      </c>
-      <c r="C16" s="8"/>
+        <v>82.72</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0.56</v>
+      </c>
       <c r="D16" s="2"/>
     </row>
     <row r="17">
@@ -628,9 +630,11 @@
         <v>18</v>
       </c>
       <c r="B17" s="5">
-        <v>10.0</v>
-      </c>
-      <c r="C17" s="8"/>
+        <v>84.01</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0.52</v>
+      </c>
       <c r="D17" s="2"/>
     </row>
     <row r="18">
@@ -638,9 +642,11 @@
         <v>19</v>
       </c>
       <c r="B18" s="5">
-        <v>10.0</v>
-      </c>
-      <c r="C18" s="8"/>
+        <v>84.06</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0.49</v>
+      </c>
       <c r="D18" s="2"/>
     </row>
     <row r="19">
@@ -648,9 +654,11 @@
         <v>20</v>
       </c>
       <c r="B19" s="5">
-        <v>10.0</v>
-      </c>
-      <c r="C19" s="8"/>
+        <v>75.74</v>
+      </c>
+      <c r="C19" s="5">
+        <v>1.21</v>
+      </c>
       <c r="D19" s="2"/>
     </row>
     <row r="20">
@@ -658,9 +666,11 @@
         <v>21</v>
       </c>
       <c r="B20" s="5">
-        <v>10.0</v>
-      </c>
-      <c r="C20" s="8"/>
+        <v>60.01</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1.28</v>
+      </c>
       <c r="D20" s="2"/>
     </row>
     <row r="21">

</xml_diff>